<commit_message>
added clients, removed social section, added disclaimer, terms n conditions, privacy policy
</commit_message>
<xml_diff>
--- a/content/Website Content.xlsx
+++ b/content/Website Content.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="70">
   <si>
     <t>Home page Content</t>
   </si>
@@ -353,12 +353,38 @@
     <t>Contents of this website are the exclusive property of Advent Global and may not be reproduced in any form without the prior written consent of Advent Global. Contents of this websites – including logos, graphics, sounds, images, and layout – are protected by trade dress, trademark, unfair competition and other laws.
 This site contains logos and trademarks of other organizations that are partners or customers of Advent Global. Terms of use for such content is solely governed by their respective owners only.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Page Description </t>
+  </si>
+  <si>
+    <t>This description would be displayed in google search result page. It should describe the page and contain keywords that  a user might use in the google search bar. Characters should be between 135 to 160.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Description
+</t>
+  </si>
+  <si>
+    <t>Page Description</t>
+  </si>
+  <si>
+    <t>Keywords that would help our page show up when searched on google.</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Advent, Solutions, Texas, Staffing, Minority, business, enterprise, contingent, workforce</t>
+  </si>
+  <si>
+    <t>Advent Global Solutions Inc. ... Advent is dedicated to delivering innovative, real-world solutions that enable our customers to tackle the toughest challenges.
+****Our current website home page description. Its 159 characters long including white space.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,6 +436,12 @@
       <i/>
       <sz val="16"/>
       <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -513,7 +545,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -582,26 +614,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -662,11 +674,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -678,25 +778,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -714,125 +796,269 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1135,10 +1361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,483 +1378,761 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="90"/>
+      <c r="B4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="50" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="90"/>
+      <c r="B5" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="90"/>
+      <c r="B6" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="51"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="90"/>
+      <c r="B7" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="17" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="52" t="s">
         <v>43</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="90"/>
+      <c r="B8" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="50" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="90"/>
+      <c r="B9" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="43"/>
+      <c r="D9" s="53" t="s">
         <v>53</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="90"/>
+      <c r="B10" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="43" t="s">
+      <c r="A11" s="90"/>
+      <c r="B11" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="54"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="183" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="87"/>
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="43"/>
+      <c r="A13" s="90"/>
+      <c r="B13" s="87"/>
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="8" t="s">
+    <row r="14" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="90"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="55" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+    <row r="15" spans="1:5" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="90"/>
+      <c r="B15" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>63</v>
+      </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="202.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:5" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="91"/>
+      <c r="B16" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="20" t="s">
+      <c r="B18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" ht="232.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="21"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="253.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="93"/>
+      <c r="B19" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="44"/>
+      <c r="D19" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="94"/>
+      <c r="B20" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="13"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27" t="s">
-        <v>43</v>
-      </c>
+    <row r="22" spans="1:5" ht="232.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="95" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="12"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="96"/>
+      <c r="B23" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="44"/>
+      <c r="D23" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="97"/>
+      <c r="B24" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="13"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+    <row r="26" spans="1:5" ht="253.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="58"/>
+      <c r="B27" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="47"/>
+      <c r="D27" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="16"/>
+    </row>
+    <row r="28" spans="1:5" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="59"/>
+      <c r="B28" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="33"/>
+      <c r="D28" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="16"/>
+    </row>
+    <row r="29" spans="1:5" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="61"/>
+      <c r="B31" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="46"/>
+      <c r="D31" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="16"/>
+    </row>
+    <row r="32" spans="1:5" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="62"/>
+      <c r="B32" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="32"/>
+      <c r="D32" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="16"/>
+    </row>
+    <row r="33" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="64"/>
+      <c r="B35" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="44"/>
+      <c r="D35" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="16"/>
+    </row>
+    <row r="36" spans="1:5" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="65"/>
+      <c r="B36" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="30"/>
+      <c r="D36" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="16"/>
+    </row>
+    <row r="37" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B38" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C38" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="29"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="2" t="s">
+      <c r="D38" s="12"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="67"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" ht="201" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="2" t="s">
+      <c r="D39" s="10"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" ht="201" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="67"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="280.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="8" t="s">
+      <c r="D40" s="10"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" ht="264.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="67"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" ht="206.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="31" t="s">
+      <c r="D41" s="10"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="67"/>
+      <c r="B42" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="44"/>
+      <c r="D42" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" s="16"/>
+    </row>
+    <row r="43" spans="1:5" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="68"/>
+      <c r="B43" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="30"/>
+      <c r="D43" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="16"/>
+    </row>
+    <row r="44" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B45" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C45" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" ht="210.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="33" t="s">
+      <c r="D45" s="12"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="70"/>
+      <c r="B46" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="45"/>
+      <c r="D46" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" s="16"/>
+    </row>
+    <row r="47" spans="1:5" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="71"/>
+      <c r="B47" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="35"/>
+      <c r="D47" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" s="16"/>
+    </row>
+    <row r="48" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B49" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C49" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="34" t="s">
+      <c r="D49" s="12"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="76"/>
+      <c r="B50" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="45"/>
+      <c r="D50" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50" s="16"/>
+    </row>
+    <row r="51" spans="1:5" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="77"/>
+      <c r="B51" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="35"/>
+      <c r="D51" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" s="16"/>
+    </row>
+    <row r="52" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B53" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C53" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D53" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="1:5" ht="137.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="35" t="s">
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="79"/>
+      <c r="B54" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="45"/>
+      <c r="D54" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E54" s="16"/>
+    </row>
+    <row r="55" spans="1:5" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="80"/>
+      <c r="B55" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="35"/>
+      <c r="D55" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55" s="16"/>
+    </row>
+    <row r="56" spans="1:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B57" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C57" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:5" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="49" t="s">
+      <c r="D57" s="12"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="82"/>
+      <c r="B58" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="44"/>
+      <c r="D58" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="E58" s="16"/>
+    </row>
+    <row r="59" spans="1:5" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="83"/>
+      <c r="B59" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" s="30"/>
+      <c r="D59" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E59" s="16"/>
+    </row>
+    <row r="60" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="50" t="s">
+      <c r="B61" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="51" t="s">
+      <c r="C61" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="52" t="s">
+      <c r="D61" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="53"/>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" ht="270.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="54" t="s">
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="73"/>
+      <c r="B62" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="27"/>
+      <c r="D62" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="16"/>
+    </row>
+    <row r="63" spans="1:5" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="74"/>
+      <c r="B63" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="40"/>
+      <c r="D63" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E63" s="16"/>
+    </row>
+    <row r="64" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="20"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" ht="270.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B65" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C65" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="55" t="s">
+      <c r="D65" s="22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="48"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-    </row>
-    <row r="43" spans="1:5" ht="244.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="54" t="s">
+    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="17"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+    </row>
+    <row r="67" spans="1:4" ht="244.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="50" t="s">
+      <c r="B67" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="51" t="s">
+      <c r="C67" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="55" t="s">
+      <c r="D67" s="22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="48"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-    </row>
-    <row r="45" spans="1:5" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="54" t="s">
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="17"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+    </row>
+    <row r="69" spans="1:4" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B69" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="51" t="s">
+      <c r="C69" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D45" s="55" t="s">
+      <c r="D69" s="22" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A27"/>
+  <mergeCells count="14">
     <mergeCell ref="B11:B14"/>
-    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="A45:A47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>